<commit_message>
Intermediate commit : solution of variable length coding bit deficit in progress.
</commit_message>
<xml_diff>
--- a/docs/count_2D_configs.xlsx
+++ b/docs/count_2D_configs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/projects/genelife/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EBB6F1-A4CD-5B4E-954E-922CFA869613}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E1FF84-4A6F-C243-A8E8-A320B5E3FB5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="3380" windowWidth="28040" windowHeight="17440" xr2:uid="{8C8B945B-6AFA-D84D-97AD-9151BA609137}"/>
+    <workbookView xWindow="7840" yWindow="2560" windowWidth="28040" windowHeight="17440" xr2:uid="{8C8B945B-6AFA-D84D-97AD-9151BA609137}"/>
   </bookViews>
   <sheets>
     <sheet name="sum 5-2 sort" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>E</t>
   </si>
@@ -101,6 +101,30 @@
   </si>
   <si>
     <t>possibly consider</t>
+  </si>
+  <si>
+    <t>birth</t>
+  </si>
+  <si>
+    <t>survival</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>values inclusive</t>
+  </si>
+  <si>
+    <t>survival configs</t>
+  </si>
+  <si>
+    <t>birth configs</t>
+  </si>
+  <si>
+    <t>1024 possibilities</t>
   </si>
 </sst>
 </file>
@@ -531,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2757C59-9D7C-1146-B512-3B386CAEC43B}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,7 +970,7 @@
         <v>5.2426406871192857</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>5</v>
       </c>
@@ -975,7 +999,7 @@
         <v>5.4142135623730949</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -1004,7 +1028,7 @@
         <v>5.6568542494923806</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>5</v>
       </c>
@@ -1033,7 +1057,7 @@
         <v>5.8284271247461898</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1062,7 +1086,7 @@
         <v>6.2426406871192857</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>5</v>
       </c>
@@ -1091,7 +1115,7 @@
         <v>6.6568542494923815</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>5</v>
       </c>
@@ -1118,6 +1142,212 @@
       <c r="H22" s="3">
         <f>G22*A22</f>
         <v>7.0710678118654755</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D25" s="3">
+        <f>H5</f>
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <f>H6</f>
+        <v>2.4142135623730949</v>
+      </c>
+      <c r="F25" s="3">
+        <f>H7</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="G25" s="3">
+        <f>H8</f>
+        <v>3</v>
+      </c>
+      <c r="H25" s="3">
+        <f>H9</f>
+        <v>3.4142135623730949</v>
+      </c>
+      <c r="I25" s="3">
+        <f>H10</f>
+        <v>3.8284271247461907</v>
+      </c>
+      <c r="J25" s="3">
+        <f>H11</f>
+        <v>4</v>
+      </c>
+      <c r="K25" s="3">
+        <f>H12</f>
+        <v>4.2426406871192857</v>
+      </c>
+      <c r="L25" s="3">
+        <f>H13</f>
+        <v>4.4142135623730949</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="M30">
+        <f>SUM(D30:L30)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
+      </c>
+      <c r="M31">
+        <f>SUM(D31:L31)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M33" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed caption information for mouse dragging for colorfunction 11,12 : now reports correctly on golb,golr respectively. Updated ppt and doc.
</commit_message>
<xml_diff>
--- a/docs/count_2D_configs.xlsx
+++ b/docs/count_2D_configs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/projects/genelife/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E1FF84-4A6F-C243-A8E8-A320B5E3FB5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E2544A-E94F-7345-89C1-12F08A9F2EBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="2560" windowWidth="28040" windowHeight="17440" xr2:uid="{8C8B945B-6AFA-D84D-97AD-9151BA609137}"/>
+    <workbookView xWindow="16720" yWindow="3280" windowWidth="28040" windowHeight="17440" xr2:uid="{8C8B945B-6AFA-D84D-97AD-9151BA609137}"/>
   </bookViews>
   <sheets>
     <sheet name="sum 5-2 sort" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -73,9 +79,6 @@
     <t>GoL LUT Analysis</t>
   </si>
   <si>
-    <t>3D</t>
-  </si>
-  <si>
     <t>2,0</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>1024 possibilities</t>
+  </si>
+  <si>
+    <t>2D</t>
   </si>
 </sst>
 </file>
@@ -558,7 +564,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +574,7 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -576,7 +582,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
@@ -618,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -630,15 +636,15 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f>SQRT(2)</f>
+        <f t="shared" ref="F5:F22" si="0">SQRT(2)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="G5" s="3">
-        <f>(C5*E5+D5*F5)/A5</f>
+        <f t="shared" ref="G5:G22" si="1">(C5*E5+D5*F5)/A5</f>
         <v>1</v>
       </c>
       <c r="H5" s="3">
-        <f>G5*A5</f>
+        <f t="shared" ref="H5:H22" si="2">G5*A5</f>
         <v>2</v>
       </c>
     </row>
@@ -647,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -659,15 +665,15 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G6" s="3">
-        <f>(C6*E6+D6*F6)/A6</f>
+        <f t="shared" si="1"/>
         <v>1.2071067811865475</v>
       </c>
       <c r="H6" s="3">
-        <f>G6*A6</f>
+        <f t="shared" si="2"/>
         <v>2.4142135623730949</v>
       </c>
     </row>
@@ -676,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
@@ -688,19 +694,19 @@
         <v>1</v>
       </c>
       <c r="F7" s="7">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G7" s="8">
-        <f>(C7*E7+D7*F7)/A7</f>
+        <f t="shared" si="1"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H7" s="8">
-        <f>G7*A7</f>
+        <f t="shared" si="2"/>
         <v>2.8284271247461903</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -708,7 +714,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="12">
         <v>3</v>
@@ -720,15 +726,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="12">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G8" s="13">
-        <f>(C8*E8+D8*F8)/A8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H8" s="13">
-        <f>G8*A8</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -737,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="12">
         <v>2</v>
@@ -749,15 +755,15 @@
         <v>1</v>
       </c>
       <c r="F9" s="12">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G9" s="13">
-        <f>(C9*E9+D9*F9)/A9</f>
+        <f t="shared" si="1"/>
         <v>1.1380711874576983</v>
       </c>
       <c r="H9" s="13">
-        <f>G9*A9</f>
+        <f t="shared" si="2"/>
         <v>3.4142135623730949</v>
       </c>
     </row>
@@ -766,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
@@ -778,15 +784,15 @@
         <v>1</v>
       </c>
       <c r="F10" s="12">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G10" s="13">
-        <f>(C10*E10+D10*F10)/A10</f>
+        <f t="shared" si="1"/>
         <v>1.2761423749153968</v>
       </c>
       <c r="H10" s="13">
-        <f>G10*A10</f>
+        <f t="shared" si="2"/>
         <v>3.8284271247461907</v>
       </c>
     </row>
@@ -807,19 +813,19 @@
         <v>1</v>
       </c>
       <c r="F11" s="15">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G11" s="16">
-        <f>(C11*E11+D11*F11)/A11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H11" s="16">
-        <f>G11*A11</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -827,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="12">
         <v>0</v>
@@ -839,15 +845,15 @@
         <v>1</v>
       </c>
       <c r="F12" s="12">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G12" s="13">
-        <f>(C12*E12+D12*F12)/A12</f>
+        <f t="shared" si="1"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H12" s="13">
-        <f>G12*A12</f>
+        <f t="shared" si="2"/>
         <v>4.2426406871192857</v>
       </c>
     </row>
@@ -868,19 +874,19 @@
         <v>1</v>
       </c>
       <c r="F13" s="7">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G13" s="8">
-        <f>(C13*E13+D13*F13)/A13</f>
+        <f t="shared" si="1"/>
         <v>1.1035533905932737</v>
       </c>
       <c r="H13" s="8">
-        <f>G13*A13</f>
+        <f t="shared" si="2"/>
         <v>4.4142135623730949</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -900,15 +906,15 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G14" s="3">
-        <f>(C14*E14+D14*F14)/A14</f>
+        <f t="shared" si="1"/>
         <v>1.2071067811865475</v>
       </c>
       <c r="H14" s="3">
-        <f>G14*A14</f>
+        <f t="shared" si="2"/>
         <v>4.8284271247461898</v>
       </c>
     </row>
@@ -929,15 +935,15 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G15" s="3">
-        <f>(C15*E15+D15*F15)/A15</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H15" s="3">
-        <f>G15*A15</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -958,15 +964,15 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G16" s="3">
-        <f>(C16*E16+D16*F16)/A16</f>
+        <f t="shared" si="1"/>
         <v>1.3106601717798214</v>
       </c>
       <c r="H16" s="3">
-        <f>G16*A16</f>
+        <f t="shared" si="2"/>
         <v>5.2426406871192857</v>
       </c>
     </row>
@@ -987,15 +993,15 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G17" s="3">
-        <f>(C17*E17+D17*F17)/A17</f>
+        <f t="shared" si="1"/>
         <v>1.0828427124746189</v>
       </c>
       <c r="H17" s="3">
-        <f>G17*A17</f>
+        <f t="shared" si="2"/>
         <v>5.4142135623730949</v>
       </c>
     </row>
@@ -1016,15 +1022,15 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G18" s="3">
-        <f>(C18*E18+D18*F18)/A18</f>
+        <f t="shared" si="1"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H18" s="3">
-        <f>G18*A18</f>
+        <f t="shared" si="2"/>
         <v>5.6568542494923806</v>
       </c>
     </row>
@@ -1045,15 +1051,15 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G19" s="3">
-        <f>(C19*E19+D19*F19)/A19</f>
+        <f t="shared" si="1"/>
         <v>1.1656854249492379</v>
       </c>
       <c r="H19" s="3">
-        <f>G19*A19</f>
+        <f t="shared" si="2"/>
         <v>5.8284271247461898</v>
       </c>
     </row>
@@ -1074,15 +1080,15 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G20" s="3">
-        <f>(C20*E20+D20*F20)/A20</f>
+        <f t="shared" si="1"/>
         <v>1.248528137423857</v>
       </c>
       <c r="H20" s="3">
-        <f>G20*A20</f>
+        <f t="shared" si="2"/>
         <v>6.2426406871192857</v>
       </c>
     </row>
@@ -1103,15 +1109,15 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G21" s="3">
-        <f>(C21*E21+D21*F21)/A21</f>
+        <f t="shared" si="1"/>
         <v>1.3313708498984762</v>
       </c>
       <c r="H21" s="3">
-        <f>G21*A21</f>
+        <f t="shared" si="2"/>
         <v>6.6568542494923815</v>
       </c>
     </row>
@@ -1132,21 +1138,21 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <f>SQRT(2)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="G22" s="3">
-        <f>(C22*E22+D22*F22)/A22</f>
+        <f t="shared" si="1"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="H22" s="3">
-        <f>G22*A22</f>
+        <f t="shared" si="2"/>
         <v>7.0710678118654755</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1189,10 +1195,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
         <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1215,7 +1221,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1241,10 +1247,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1267,7 +1273,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1293,7 +1299,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30">
         <v>7</v>
@@ -1320,7 +1326,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E31">
         <v>7</v>
@@ -1347,11 +1353,11 @@
     </row>
     <row r="33" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A5:H22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H22">
     <sortCondition ref="H5:H22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1378,10 +1384,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>2</v>
@@ -1621,10 +1627,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>2</v>
@@ -1835,10 +1841,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>2</v>
@@ -1871,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1900,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1929,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1958,7 +1964,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2020,10 +2026,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>2</v>
@@ -2056,7 +2062,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2085,7 +2091,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2114,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>1</v>

</xml_diff>